<commit_message>
Update Data Analysis file. Update data from experiment.
</commit_message>
<xml_diff>
--- a/Data/RP4, 11-6-23.xlsx
+++ b/Data/RP4, 11-6-23.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11008"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/apiskadlo/Documents/All Work/U of U/2023 School/Fall 2023/Neural Engineering and NeurorRbotics/Labs/NENR_Project 4/NENR_Project4/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Github\NENR_Project4\Data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9AF9F4B4-1DDC-4D4A-AC7C-54C00821DF58}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E13044B7-E248-4E23-A333-0A14E3EA3353}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="35840" yWindow="-520" windowWidth="38400" windowHeight="21100" activeTab="1" xr2:uid="{9AB512DC-2A16-A146-BDF8-FB3A09F62B78}"/>
+    <workbookView xWindow="-90" yWindow="0" windowWidth="14835" windowHeight="15480" activeTab="2" xr2:uid="{9AB512DC-2A16-A146-BDF8-FB3A09F62B78}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
     <sheet name="Sheet2" sheetId="2" r:id="rId2"/>
+    <sheet name="WMM" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +38,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="125" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="45">
   <si>
     <t>Andrew Piskadlo</t>
   </si>
@@ -169,6 +170,9 @@
   </si>
   <si>
     <t>Measured from the halfway point of phalangires</t>
+  </si>
+  <si>
+    <t>t (us):</t>
   </si>
 </sst>
 </file>
@@ -1711,20 +1715,20 @@
       <selection activeCell="D52" sqref="D51:D52"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="3" max="3" width="19.33203125" customWidth="1"/>
-    <col min="4" max="4" width="15.6640625" customWidth="1"/>
-    <col min="5" max="5" width="16.33203125" customWidth="1"/>
-    <col min="9" max="14" width="15.6640625" customWidth="1"/>
+    <col min="3" max="3" width="19.375" customWidth="1"/>
+    <col min="4" max="4" width="15.625" customWidth="1"/>
+    <col min="5" max="5" width="16.375" customWidth="1"/>
+    <col min="9" max="14" width="15.625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>1</v>
       </c>
@@ -1732,12 +1736,12 @@
         <v>4</v>
       </c>
     </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="I3" t="s">
         <v>14</v>
       </c>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>2</v>
       </c>
@@ -1748,7 +1752,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>3</v>
       </c>
@@ -1771,7 +1775,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B6">
         <v>1</v>
       </c>
@@ -1806,7 +1810,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B7">
         <v>2</v>
       </c>
@@ -1838,7 +1842,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B8">
         <v>3</v>
       </c>
@@ -1870,7 +1874,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B9">
         <v>4</v>
       </c>
@@ -1902,7 +1906,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B10">
         <v>5</v>
       </c>
@@ -1937,7 +1941,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B11">
         <v>6</v>
       </c>
@@ -1972,7 +1976,7 @@
         <v>22</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B12">
         <v>7</v>
       </c>
@@ -2007,7 +2011,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B13">
         <v>8</v>
       </c>
@@ -2039,7 +2043,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B14">
         <v>9</v>
       </c>
@@ -2071,7 +2075,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B15">
         <v>10</v>
       </c>
@@ -2103,7 +2107,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="B16">
         <v>11</v>
       </c>
@@ -2135,7 +2139,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="17" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B17">
         <v>12</v>
       </c>
@@ -2167,7 +2171,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="18" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B18">
         <v>13</v>
       </c>
@@ -2181,7 +2185,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="19" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B19">
         <v>14</v>
       </c>
@@ -2195,7 +2199,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="20" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B20">
         <v>15</v>
       </c>
@@ -2215,7 +2219,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="21" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B21">
         <v>16</v>
       </c>
@@ -2235,7 +2239,7 @@
         <v>200</v>
       </c>
     </row>
-    <row r="22" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B22" s="2">
         <v>16</v>
       </c>
@@ -2258,7 +2262,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B23">
         <v>17</v>
       </c>
@@ -2281,7 +2285,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="24" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B24">
         <v>18</v>
       </c>
@@ -2304,7 +2308,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B25">
         <v>19</v>
       </c>
@@ -2318,7 +2322,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="26" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B26">
         <v>20</v>
       </c>
@@ -2332,7 +2336,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="27" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B27">
         <v>21</v>
       </c>
@@ -2346,7 +2350,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="28" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B28">
         <v>22</v>
       </c>
@@ -2360,7 +2364,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="29" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B29">
         <v>23</v>
       </c>
@@ -2374,7 +2378,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="30" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B30">
         <v>24</v>
       </c>
@@ -2388,7 +2392,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="31" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B31">
         <v>25</v>
       </c>
@@ -2402,7 +2406,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="32" spans="2:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="2:14" x14ac:dyDescent="0.25">
       <c r="B32">
         <v>26</v>
       </c>
@@ -2416,7 +2420,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="33" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B33">
         <v>27</v>
       </c>
@@ -2430,7 +2434,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="34" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B34">
         <v>28</v>
       </c>
@@ -2444,7 +2448,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="35" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B35">
         <v>29</v>
       </c>
@@ -2458,7 +2462,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="36" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="36" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B36">
         <v>30</v>
       </c>
@@ -2472,7 +2476,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C37">
         <v>1.7</v>
       </c>
@@ -2483,7 +2487,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="38" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="38" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C38">
         <v>1.7</v>
       </c>
@@ -2494,7 +2498,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C39">
         <v>1.7</v>
       </c>
@@ -2505,7 +2509,7 @@
         <v>8</v>
       </c>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:5" x14ac:dyDescent="0.25">
       <c r="C40">
         <v>5</v>
       </c>
@@ -2516,12 +2520,12 @@
         <v>10</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.25">
       <c r="E42" t="s">
         <v>13</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.25">
       <c r="B43" t="s">
         <v>12</v>
       </c>
@@ -2546,24 +2550,24 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BAAD2FAE-853B-AA4E-99AF-C94460638C4E}">
   <dimension ref="A1:G20"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="E1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E7" sqref="E7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="2" max="2" width="12" customWidth="1"/>
     <col min="4" max="4" width="12.5" customWidth="1"/>
     <col min="5" max="5" width="14.5" customWidth="1"/>
-    <col min="6" max="7" width="12.1640625" customWidth="1"/>
+    <col min="6" max="7" width="12.125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
         <v>25</v>
       </c>
@@ -2574,7 +2578,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
         <v>26</v>
       </c>
@@ -2594,7 +2598,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
         <v>27</v>
       </c>
@@ -2611,7 +2615,7 @@
         <v>300</v>
       </c>
     </row>
-    <row r="5" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>29</v>
       </c>
@@ -2622,17 +2626,17 @@
         <v>30</v>
       </c>
     </row>
-    <row r="6" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="E6" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="D7" t="s">
         <v>42</v>
       </c>
     </row>
-    <row r="8" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A8" s="13" t="s">
         <v>36</v>
       </c>
@@ -2652,7 +2656,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="9" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="10">
         <v>1</v>
       </c>
@@ -2670,7 +2674,7 @@
       </c>
       <c r="F9" s="12"/>
     </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="5">
         <v>2</v>
       </c>
@@ -2688,7 +2692,7 @@
       </c>
       <c r="F10" s="6"/>
     </row>
-    <row r="11" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A11" s="7">
         <v>3</v>
       </c>
@@ -2706,7 +2710,7 @@
       </c>
       <c r="F11" s="9"/>
     </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="10">
         <v>4</v>
       </c>
@@ -2722,7 +2726,7 @@
       <c r="E12" s="11"/>
       <c r="F12" s="12"/>
     </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="5">
         <v>5</v>
       </c>
@@ -2738,7 +2742,7 @@
       <c r="E13" s="4"/>
       <c r="F13" s="6"/>
     </row>
-    <row r="14" spans="1:7" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A14" s="7">
         <v>6</v>
       </c>
@@ -2754,7 +2758,7 @@
       <c r="E14" s="8"/>
       <c r="F14" s="9"/>
     </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="10">
         <v>7</v>
       </c>
@@ -2770,7 +2774,7 @@
       <c r="E15" s="11"/>
       <c r="F15" s="12"/>
     </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="5">
         <v>8</v>
       </c>
@@ -2786,7 +2790,7 @@
       <c r="E16" s="4"/>
       <c r="F16" s="6"/>
     </row>
-    <row r="17" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A17" s="7">
         <v>9</v>
       </c>
@@ -2802,7 +2806,7 @@
       <c r="E17" s="8"/>
       <c r="F17" s="9"/>
     </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A18" s="10">
         <v>10</v>
       </c>
@@ -2816,7 +2820,7 @@
       <c r="E18" s="11"/>
       <c r="F18" s="12"/>
     </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
       <c r="A19" s="5">
         <v>11</v>
       </c>
@@ -2830,7 +2834,7 @@
       <c r="E19" s="4"/>
       <c r="F19" s="6"/>
     </row>
-    <row r="20" spans="1:6" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A20" s="7">
         <v>12</v>
       </c>
@@ -2843,6 +2847,355 @@
       <c r="D20" s="19"/>
       <c r="E20" s="8"/>
       <c r="F20" s="9"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AD78D402-14DD-42EE-AB12-6A07F4F5282B}">
+  <dimension ref="A1:G20"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="2" max="2" width="12" customWidth="1"/>
+    <col min="4" max="4" width="12.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" customWidth="1"/>
+    <col min="6" max="7" width="12.125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F2" t="s">
+        <v>32</v>
+      </c>
+      <c r="G2" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A3" t="s">
+        <v>44</v>
+      </c>
+      <c r="B3">
+        <v>250</v>
+      </c>
+      <c r="C3" t="s">
+        <v>28</v>
+      </c>
+      <c r="E3" t="s">
+        <v>34</v>
+      </c>
+      <c r="F3">
+        <v>5</v>
+      </c>
+      <c r="G3">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B4">
+        <v>30</v>
+      </c>
+      <c r="E4" t="s">
+        <v>33</v>
+      </c>
+      <c r="F4">
+        <v>150</v>
+      </c>
+      <c r="G4">
+        <v>300</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A5" t="s">
+        <v>29</v>
+      </c>
+      <c r="B5">
+        <v>3</v>
+      </c>
+      <c r="C5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="E6" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="D7" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A8" s="13" t="s">
+        <v>36</v>
+      </c>
+      <c r="B8" s="14" t="s">
+        <v>35</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>38</v>
+      </c>
+      <c r="D8" s="16" t="s">
+        <v>37</v>
+      </c>
+      <c r="E8" s="14" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="15" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A9" s="10">
+        <v>1</v>
+      </c>
+      <c r="B9" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C9" s="12">
+        <v>1</v>
+      </c>
+      <c r="D9" s="17">
+        <v>1.7</v>
+      </c>
+      <c r="E9" s="11">
+        <v>1</v>
+      </c>
+      <c r="F9" s="12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" s="5">
+        <v>2</v>
+      </c>
+      <c r="B10" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C10" s="6">
+        <v>2</v>
+      </c>
+      <c r="D10" s="18">
+        <v>1.4</v>
+      </c>
+      <c r="E10" s="4">
+        <v>0.5</v>
+      </c>
+      <c r="F10" s="6">
+        <v>0.8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A11" s="7">
+        <v>3</v>
+      </c>
+      <c r="B11" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C11" s="9">
+        <v>3</v>
+      </c>
+      <c r="D11" s="19">
+        <v>1.4</v>
+      </c>
+      <c r="E11" s="8">
+        <v>1</v>
+      </c>
+      <c r="F11" s="9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" s="10">
+        <v>4</v>
+      </c>
+      <c r="B12" s="11" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" s="12">
+        <v>1</v>
+      </c>
+      <c r="D12" s="17">
+        <v>0.9</v>
+      </c>
+      <c r="E12" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F12" s="12">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" s="5">
+        <v>5</v>
+      </c>
+      <c r="B13" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" s="6">
+        <v>2</v>
+      </c>
+      <c r="D13" s="18">
+        <v>1</v>
+      </c>
+      <c r="E13" s="4">
+        <v>1</v>
+      </c>
+      <c r="F13" s="6">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A14" s="7">
+        <v>6</v>
+      </c>
+      <c r="B14" s="8" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" s="9">
+        <v>3</v>
+      </c>
+      <c r="D14" s="19">
+        <v>1.25</v>
+      </c>
+      <c r="E14" s="8">
+        <v>0.5</v>
+      </c>
+      <c r="F14" s="9">
+        <v>0.4</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" s="10">
+        <v>7</v>
+      </c>
+      <c r="B15" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="17">
+        <v>3.3</v>
+      </c>
+      <c r="E15" s="11">
+        <v>0.6</v>
+      </c>
+      <c r="F15" s="12">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" s="5">
+        <v>8</v>
+      </c>
+      <c r="B16" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C16" s="6">
+        <v>2</v>
+      </c>
+      <c r="D16" s="18">
+        <v>4.5</v>
+      </c>
+      <c r="E16" s="4">
+        <v>1.1000000000000001</v>
+      </c>
+      <c r="F16" s="6">
+        <v>1.9</v>
+      </c>
+    </row>
+    <row r="17" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A17" s="7">
+        <v>9</v>
+      </c>
+      <c r="B17" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" s="9">
+        <v>3</v>
+      </c>
+      <c r="D17" s="19">
+        <v>4.8</v>
+      </c>
+      <c r="E17" s="8">
+        <v>1.2</v>
+      </c>
+      <c r="F17" s="9">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A18" s="10">
+        <v>10</v>
+      </c>
+      <c r="B18" s="11" t="s">
+        <v>12</v>
+      </c>
+      <c r="C18" s="12">
+        <v>1</v>
+      </c>
+      <c r="D18" s="17"/>
+      <c r="E18" s="11">
+        <v>0.5</v>
+      </c>
+      <c r="F18" s="12">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="A19" s="5">
+        <v>11</v>
+      </c>
+      <c r="B19" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="C19" s="6">
+        <v>2</v>
+      </c>
+      <c r="D19" s="18"/>
+      <c r="E19" s="4">
+        <v>0.4</v>
+      </c>
+      <c r="F19" s="6">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="20" spans="1:6" ht="16.5" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A20" s="7">
+        <v>12</v>
+      </c>
+      <c r="B20" s="8" t="s">
+        <v>12</v>
+      </c>
+      <c r="C20" s="9">
+        <v>3</v>
+      </c>
+      <c r="D20" s="19"/>
+      <c r="E20" s="8">
+        <v>0.4</v>
+      </c>
+      <c r="F20" s="9">
+        <v>1.2</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>